<commit_message>
aplicando logica de cadastro
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">Nome Completo</t>
   </si>
@@ -28,12 +28,18 @@
     <t xml:space="preserve">Telefone</t>
   </si>
   <si>
+    <t xml:space="preserve">Ativo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eugenio</t>
   </si>
   <si>
     <t xml:space="preserve">5511940502208</t>
   </si>
   <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gustavo</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">5511944400392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -146,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -166,29 +175,41 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluindo variacao de img
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">Nome Completo</t>
   </si>
@@ -31,19 +31,22 @@
     <t xml:space="preserve">Ativo</t>
   </si>
   <si>
-    <t xml:space="preserve">Eugenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5511940502208</t>
+    <t xml:space="preserve">Arquivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5511943808142</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">Gustavo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5511963943402</t>
+    <t xml:space="preserve">Pietra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5511941900392</t>
   </si>
   <si>
     <t xml:space="preserve">Juliana</t>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teste.jpg</t>
   </si>
 </sst>
 </file>
@@ -155,10 +161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -178,38 +184,44 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>